<commit_message>
Changes to Gantt Chart
</commit_message>
<xml_diff>
--- a/Milestone 2 - Team 7 - Gantt chart.xlsx
+++ b/Milestone 2 - Team 7 - Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mary/Documents/Fall21/CMPE131/Team-7/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF09E1BA-E54A-004A-932C-4BECF44BEEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10164"/>
+    <workbookView xWindow="7140" yWindow="1360" windowWidth="23040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>PERIODS</t>
   </si>
@@ -181,12 +182,33 @@
   <si>
     <t>Team 7 Project Planner</t>
   </si>
+  <si>
+    <t>User Login/Signup/Delete Account</t>
+  </si>
+  <si>
+    <t>Use Case 10: Add Tags to notes</t>
+  </si>
+  <si>
+    <t>Use Case 11: Add flashcards to mind map</t>
+  </si>
+  <si>
+    <t>Use Case 12: Share flashcards with other people</t>
+  </si>
+  <si>
+    <t>Use Case 13: Create pdf of flashcards to print</t>
+  </si>
+  <si>
+    <t>Use Case 14: Share notes</t>
+  </si>
+  <si>
+    <t>Use Case 15:Visualize time blocks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -294,6 +316,11 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="8">
@@ -482,7 +509,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,29 +621,1049 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="82">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -998,27 +2045,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO13"/>
+  <dimension ref="B1:BO20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.5" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="8" max="9" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="27" width="2.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
@@ -1028,7 +2076,7 @@
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
@@ -1040,7 +2088,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="14">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="29" t="s">
@@ -1086,7 +2134,7 @@
       <c r="AO2" s="22"/>
       <c r="AP2" s="22"/>
     </row>
-    <row r="3" spans="2:67" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:67" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
         <v>13</v>
       </c>
@@ -1128,7 +2176,7 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1136,218 +2184,146 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="3">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>21</v>
+      </c>
+      <c r="R4" s="3">
+        <v>22</v>
+      </c>
+      <c r="S4" s="3">
+        <v>23</v>
+      </c>
+      <c r="T4" s="3">
+        <v>24</v>
+      </c>
+      <c r="U4" s="3">
+        <v>25</v>
+      </c>
+      <c r="V4" s="3">
+        <v>26</v>
+      </c>
+      <c r="W4" s="3">
+        <v>27</v>
+      </c>
+      <c r="X4" s="3">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>30</v>
+      </c>
+      <c r="AA4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
+      <c r="AB4" s="3">
         <v>2</v>
       </c>
-      <c r="J4" s="3">
+      <c r="AC4" s="3">
         <v>3</v>
       </c>
-      <c r="K4" s="3">
+      <c r="AD4" s="3">
         <v>4</v>
       </c>
-      <c r="L4" s="3">
+      <c r="AE4" s="3">
         <v>5</v>
       </c>
-      <c r="M4" s="3">
-        <v>6</v>
-      </c>
-      <c r="N4" s="3">
-        <v>7</v>
-      </c>
-      <c r="O4" s="3">
-        <v>8</v>
-      </c>
-      <c r="P4" s="3">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>10</v>
-      </c>
-      <c r="R4" s="3">
-        <v>11</v>
-      </c>
-      <c r="S4" s="3">
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="3"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="3"/>
+      <c r="BJ4" s="3"/>
+      <c r="BK4" s="3"/>
+      <c r="BL4" s="3"/>
+      <c r="BM4" s="3"/>
+      <c r="BN4" s="3"/>
+      <c r="BO4" s="3"/>
+    </row>
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7">
         <v>12</v>
-      </c>
-      <c r="T4" s="3">
-        <v>13</v>
-      </c>
-      <c r="U4" s="3">
-        <v>14</v>
-      </c>
-      <c r="V4" s="3">
-        <v>15</v>
-      </c>
-      <c r="W4" s="3">
-        <v>16</v>
-      </c>
-      <c r="X4" s="3">
-        <v>17</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>18</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>19</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>20</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>21</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>22</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>23</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>24</v>
-      </c>
-      <c r="AF4" s="3">
-        <v>25</v>
-      </c>
-      <c r="AG4" s="3">
-        <v>26</v>
-      </c>
-      <c r="AH4" s="3">
-        <v>27</v>
-      </c>
-      <c r="AI4" s="3">
-        <v>28</v>
-      </c>
-      <c r="AJ4" s="3">
-        <v>29</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>30</v>
-      </c>
-      <c r="AL4" s="3">
-        <v>31</v>
-      </c>
-      <c r="AM4" s="3">
-        <v>32</v>
-      </c>
-      <c r="AN4" s="3">
-        <v>33</v>
-      </c>
-      <c r="AO4" s="3">
-        <v>34</v>
-      </c>
-      <c r="AP4" s="3">
-        <v>35</v>
-      </c>
-      <c r="AQ4" s="3">
-        <v>36</v>
-      </c>
-      <c r="AR4" s="3">
-        <v>37</v>
-      </c>
-      <c r="AS4" s="3">
-        <v>38</v>
-      </c>
-      <c r="AT4" s="3">
-        <v>39</v>
-      </c>
-      <c r="AU4" s="3">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="3">
-        <v>41</v>
-      </c>
-      <c r="AW4" s="3">
-        <v>42</v>
-      </c>
-      <c r="AX4" s="3">
-        <v>43</v>
-      </c>
-      <c r="AY4" s="3">
-        <v>44</v>
-      </c>
-      <c r="AZ4" s="3">
-        <v>45</v>
-      </c>
-      <c r="BA4" s="3">
-        <v>46</v>
-      </c>
-      <c r="BB4" s="3">
-        <v>47</v>
-      </c>
-      <c r="BC4" s="3">
-        <v>48</v>
-      </c>
-      <c r="BD4" s="3">
-        <v>49</v>
-      </c>
-      <c r="BE4" s="3">
-        <v>50</v>
-      </c>
-      <c r="BF4" s="3">
-        <v>51</v>
-      </c>
-      <c r="BG4" s="3">
-        <v>52</v>
-      </c>
-      <c r="BH4" s="3">
-        <v>53</v>
-      </c>
-      <c r="BI4" s="3">
-        <v>54</v>
-      </c>
-      <c r="BJ4" s="3">
-        <v>55</v>
-      </c>
-      <c r="BK4" s="3">
-        <v>56</v>
-      </c>
-      <c r="BL4" s="3">
-        <v>57</v>
-      </c>
-      <c r="BM4" s="3">
-        <v>58</v>
-      </c>
-      <c r="BN4" s="3">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
+        <v>13</v>
+      </c>
+      <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
       <c r="E6" s="7">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -1356,132 +2332,260 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D7" s="7">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
+      <c r="E7" s="7">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7">
         <v>3</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="7">
+        <v>25</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7">
         <v>3</v>
       </c>
       <c r="E9" s="7">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7">
-        <v>3</v>
-      </c>
-      <c r="E10" s="7">
-        <v>4</v>
-      </c>
-      <c r="F10" s="7">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="37">
+        <v>17</v>
+      </c>
+      <c r="D10" s="37">
+        <v>1</v>
+      </c>
+      <c r="E10" s="37">
+        <v>25</v>
+      </c>
+      <c r="F10" s="37">
+        <v>2</v>
       </c>
       <c r="G10" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7">
-        <v>5</v>
-      </c>
-      <c r="F11" s="7">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="37">
+        <v>17</v>
+      </c>
+      <c r="D11" s="37">
+        <v>1</v>
+      </c>
+      <c r="E11" s="37">
+        <v>25</v>
+      </c>
+      <c r="F11" s="37">
+        <v>2</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="7">
-        <v>5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7">
-        <v>6</v>
-      </c>
-      <c r="F12" s="7">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C12" s="37">
+        <v>17</v>
+      </c>
+      <c r="D12" s="37">
+        <v>1</v>
+      </c>
+      <c r="E12" s="37">
+        <v>25</v>
+      </c>
+      <c r="F12" s="37">
+        <v>4</v>
       </c>
       <c r="G12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7">
+        <v>21</v>
+      </c>
+      <c r="C13" s="37">
+        <v>12</v>
+      </c>
+      <c r="D13" s="37">
         <v>3</v>
       </c>
-      <c r="E13" s="7">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="E13" s="37">
+        <v>15</v>
+      </c>
+      <c r="F13" s="37">
         <v>5</v>
       </c>
       <c r="G13" s="8">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="37">
+        <v>12</v>
+      </c>
+      <c r="D14" s="37">
+        <v>3</v>
+      </c>
+      <c r="E14" s="37">
+        <v>15</v>
+      </c>
+      <c r="F14" s="37">
+        <v>5</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="37">
+        <v>1</v>
+      </c>
+      <c r="D15" s="37">
+        <v>3</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="37">
+        <v>1</v>
+      </c>
+      <c r="D16" s="37">
+        <v>3</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="37">
+        <v>1</v>
+      </c>
+      <c r="D17" s="37">
+        <v>3</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="37">
+        <v>1</v>
+      </c>
+      <c r="D18" s="37">
+        <v>3</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="37">
+        <v>1</v>
+      </c>
+      <c r="D19" s="37">
+        <v>3</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="37">
+        <v>1</v>
+      </c>
+      <c r="D20" s="37">
+        <v>3</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1500,61 +2604,243 @@
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="H5:BO13">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="H6:BO14">
+    <cfRule type="expression" dxfId="81" priority="73">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="80" priority="75">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="79" priority="76">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="78" priority="77">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="77" priority="78">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="76" priority="79">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="75" priority="83">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="74" priority="84">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:BO14">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="B21:BO21">
+    <cfRule type="expression" dxfId="73" priority="74">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
+    <cfRule type="expression" dxfId="72" priority="80">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:BO5">
+    <cfRule type="expression" dxfId="71" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="66">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="70">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="71">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="72">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:BO17">
+    <cfRule type="expression" dxfId="55" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="50" priority="30">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:BO15">
+    <cfRule type="expression" dxfId="47" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="46">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:BO16">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:BO19">
+    <cfRule type="expression" dxfId="31" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="14">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:BO18">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:BO20">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>